<commit_message>
adding functions to draw systems
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/parallelSystemTest.xlsx
+++ b/shipClassTests/testResults/parallelSystemTest.xlsx
@@ -393,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -796,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -874,16 +874,16 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -895,10 +895,10 @@
         <v>1</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -908,8 +908,1385 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f>IF(B11 = I11, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <f>IF(B12 = I12, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f>IF(B13 = I13, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <f>IF(B14 = I14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <f>IF(B15 = I15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <f>IF(B16 = I16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <f>IF(B17 = I17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f>IF(B18 = I18, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <f>IF(B19 = I19, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <f>IF(B20 = I20, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <f>IF(B21 = I21, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <f>IF(B22 = I22, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <f>IF(B23 = I23, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <f>IF(B24 = I24, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <f>IF(B25 = I25, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <f>IF(B26 = I26, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <f>IF(B27 = I27, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <f>IF(B28 = I28, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <f>IF(B29 = I29, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <f>IF(B30 = I30, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <f>IF(B31 = I31, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <f>IF(B32 = I32, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <f>IF(B33 = I33, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <f>IF(B34 = I34, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <f>IF(B35 = I35, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <f>IF(B36 = I36, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <f>IF(B37 = I37, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="P2:P10">
+  <conditionalFormatting sqref="P2:P37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>